<commit_message>
Fixed XML Encoding Issue : eachOutputFileData = ET.tostring(xmlTag, encoding='UTF-8', method='xml',xml_declaration=True).decode()
</commit_message>
<xml_diff>
--- a/InputResource/MasterCopyInputExcel.xlsx
+++ b/InputResource/MasterCopyInputExcel.xlsx
@@ -736,12 +736,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -893,58 +900,46 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -952,19 +947,34 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1422,7 +1432,7 @@
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1441,10 +1451,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1496,7 +1506,7 @@
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="26" t="s">
         <v>196</v>
       </c>
       <c r="D5" s="9" t="s">

</xml_diff>